<commit_message>
Grace 3rd updates 0804
</commit_message>
<xml_diff>
--- a/SDG Financing Simplified model (Egypt)/v4_commented and cleaned - for calibration/auxiliary/datainput_bot.xlsx
+++ b/SDG Financing Simplified model (Egypt)/v4_commented and cleaned - for calibration/auxiliary/datainput_bot.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="123">
   <si>
     <t>male</t>
   </si>
@@ -9236,14 +9236,210 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.725" defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.725" defaultRowHeight="13.5" outlineLevelCol="2"/>
+  <sheetData>
+    <row r="1" spans="2:3">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>0.027095304550216</v>
+      </c>
+      <c r="C2">
+        <v>0.02600645374266</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>0.0269967348904</v>
+      </c>
+      <c r="C3">
+        <v>0.025924883055</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>0.02657923282358</v>
+      </c>
+      <c r="C4">
+        <v>0.02552244412122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>0.02616173075676</v>
+      </c>
+      <c r="C5">
+        <v>0.02512000518744</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>0.02574422868994</v>
+      </c>
+      <c r="C6">
+        <v>0.02471756625366</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>0.02532672662312</v>
+      </c>
+      <c r="C7">
+        <v>0.02431512731988</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>0.0249092245563</v>
+      </c>
+      <c r="C8">
+        <v>0.0239126883861</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>0.01998235557356</v>
+      </c>
+      <c r="C9">
+        <v>0.020238378757836</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>0.01963774221982</v>
+      </c>
+      <c r="C10">
+        <v>0.019885039038852</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>0.01929312886608</v>
+      </c>
+      <c r="C11">
+        <v>0.019531699319868</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>0.01189897721506</v>
+      </c>
+      <c r="C12">
+        <v>0.0151726030368</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>0.0116825725874</v>
+      </c>
+      <c r="C13">
+        <v>0.01489306488</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14">
+        <v>0.00453967276</v>
+      </c>
+      <c r="C14">
+        <v>0.00697572612</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15">
+        <v>0.00444810352</v>
+      </c>
+      <c r="C15">
+        <v>0.00684189924</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16">
+        <v>0.00435653428</v>
+      </c>
+      <c r="C16">
+        <v>0.00670807236</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17">
+        <v>0.00426496504</v>
+      </c>
+      <c r="C17">
+        <v>0.00657424548</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18">
+        <v>0.0041733958</v>
+      </c>
+      <c r="C18">
+        <v>0.0064404186</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>